<commit_message>
Added echo "$" case
</commit_message>
<xml_diff>
--- a/test_files/tokenization/expansion.xlsx
+++ b/test_files/tokenization/expansion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brt.hawayda\Desktop\42\minishell\minishell-tester\test_files\tokenization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D67C3-13FB-4AFC-9BBA-80272A511ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0798A637-566F-404F-BC9E-BCBF51FC5741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="547">
   <si>
     <t>echo    | cat -e</t>
   </si>
@@ -1657,6 +1657,15 @@
   </si>
   <si>
     <t>echo $? &amp;&amp; echo $? || echo failed</t>
+  </si>
+  <si>
+    <t>echo $"$SHLVL"</t>
+  </si>
+  <si>
+    <t>echo $'$SHLVL'</t>
+  </si>
+  <si>
+    <t>echo "$"</t>
   </si>
 </sst>
 </file>
@@ -2123,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH383"/>
+  <dimension ref="A1:AMH386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C381" sqref="C381"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2468,43 +2477,43 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>351</v>
+        <v>546</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>349</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C32" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>408</v>
+        <v>353</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>413</v>
+        <v>354</v>
       </c>
       <c r="C33" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C34" s="1">
         <v>5</v>
@@ -2512,32 +2521,32 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>354</v>
+        <v>414</v>
       </c>
       <c r="C35" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>413</v>
+        <v>354</v>
       </c>
       <c r="C36" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C37" s="1">
         <v>5</v>
@@ -2545,21 +2554,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C38" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C39" s="1">
         <v>4</v>
@@ -2567,32 +2576,32 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>355</v>
+        <v>416</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>355</v>
+        <v>418</v>
       </c>
       <c r="C40" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -2600,10 +2609,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C43" s="1">
         <v>2</v>
@@ -2611,10 +2620,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
@@ -2622,10 +2631,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
@@ -2633,10 +2642,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
@@ -2644,10 +2653,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C47" s="1">
         <v>2</v>
@@ -2655,10 +2664,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C48" s="1">
         <v>2</v>
@@ -2666,10 +2675,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C49" s="1">
         <v>2</v>
@@ -2677,10 +2686,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C50" s="1">
         <v>2</v>
@@ -2688,10 +2697,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C51" s="1">
         <v>2</v>
@@ -2699,10 +2708,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C52" s="1">
         <v>2</v>
@@ -2710,10 +2719,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>402</v>
+        <v>376</v>
       </c>
       <c r="C53" s="1">
         <v>2</v>
@@ -2721,10 +2730,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="C54" s="1">
         <v>2</v>
@@ -2732,10 +2741,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C55" s="1">
         <v>2</v>
@@ -2743,10 +2752,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C56" s="1">
         <v>2</v>
@@ -2754,10 +2763,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C57" s="1">
         <v>2</v>
@@ -2765,10 +2774,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C58" s="1">
         <v>2</v>
@@ -2776,10 +2785,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C59" s="1">
         <v>2</v>
@@ -2787,10 +2796,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>371</v>
+        <v>386</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
       <c r="C60" s="1">
         <v>2</v>
@@ -2798,10 +2807,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C61" s="1">
         <v>2</v>
@@ -2809,10 +2818,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C62" s="1">
         <v>2</v>
@@ -2820,10 +2829,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="C63" s="1">
         <v>2</v>
@@ -2831,10 +2840,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C64" s="1">
         <v>2</v>
@@ -2842,10 +2851,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C65" s="1">
         <v>2</v>
@@ -2853,10 +2862,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>357</v>
+        <v>397</v>
       </c>
       <c r="C66" s="1">
         <v>2</v>
@@ -2864,21 +2873,21 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>401</v>
+        <v>357</v>
       </c>
       <c r="C67" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>3</v>
+        <v>401</v>
       </c>
       <c r="C68" s="1">
         <v>3</v>
@@ -2886,7 +2895,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>3</v>
@@ -2897,10 +2906,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C70" s="1">
         <v>3</v>
@@ -2908,10 +2917,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C71" s="1">
         <v>3</v>
@@ -2919,7 +2928,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>3</v>
@@ -2930,10 +2939,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" s="1">
         <v>3</v>
@@ -2941,10 +2950,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C74" s="1">
         <v>3</v>
@@ -2952,10 +2961,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C75" s="1">
         <v>3</v>
@@ -2963,7 +2972,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
@@ -2974,10 +2983,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C77" s="1">
         <v>3</v>
@@ -2985,10 +2994,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C78" s="1">
         <v>3</v>
@@ -2996,10 +3005,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C79" s="1">
         <v>3</v>
@@ -3007,7 +3016,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
@@ -3018,10 +3027,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C81" s="1">
         <v>3</v>
@@ -3029,10 +3038,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>403</v>
+        <v>2</v>
       </c>
       <c r="C82" s="1">
         <v>3</v>
@@ -3040,10 +3049,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>0</v>
+        <v>403</v>
       </c>
       <c r="C83" s="1">
         <v>3</v>
@@ -3051,7 +3060,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>0</v>
@@ -3062,7 +3071,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>0</v>
@@ -3073,7 +3082,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>0</v>
@@ -3084,10 +3093,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>403</v>
+        <v>0</v>
       </c>
       <c r="C87" s="1">
         <v>3</v>
@@ -3095,10 +3104,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>0</v>
+        <v>403</v>
       </c>
       <c r="C88" s="1">
         <v>3</v>
@@ -3106,7 +3115,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>0</v>
@@ -3117,7 +3126,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>0</v>
@@ -3128,7 +3137,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>0</v>
@@ -3139,10 +3148,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>404</v>
+        <v>0</v>
       </c>
       <c r="C92" s="1">
         <v>3</v>
@@ -3150,18 +3159,18 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C93" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>0</v>
@@ -3172,10 +3181,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C95" s="1">
         <v>4</v>
@@ -3183,7 +3192,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>3</v>
@@ -3194,10 +3203,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>404</v>
+        <v>3</v>
       </c>
       <c r="C97" s="1">
         <v>4</v>
@@ -3205,10 +3214,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C98" s="1">
         <v>4</v>
@@ -3216,7 +3225,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>0</v>
@@ -3227,10 +3236,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C100" s="1">
         <v>4</v>
@@ -3238,21 +3247,21 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C101" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>404</v>
+        <v>3</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
@@ -3260,10 +3269,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
@@ -3271,7 +3280,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>0</v>
@@ -3282,10 +3291,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
@@ -3293,7 +3302,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>3</v>
@@ -3304,10 +3313,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>404</v>
+        <v>3</v>
       </c>
       <c r="C107" s="1">
         <v>1</v>
@@ -3315,10 +3324,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
@@ -3326,7 +3335,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>0</v>
@@ -3337,10 +3346,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
@@ -3348,7 +3357,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>3</v>
@@ -3359,10 +3368,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
@@ -3370,10 +3379,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -3381,7 +3390,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>3</v>
@@ -3392,10 +3401,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -3403,10 +3412,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
@@ -3414,10 +3423,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
@@ -3425,7 +3434,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>5</v>
@@ -3436,10 +3445,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
@@ -3447,10 +3456,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C120" s="1">
         <v>1</v>
@@ -3458,10 +3467,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C121" s="1">
         <v>1</v>
@@ -3469,7 +3478,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>5</v>
@@ -3480,10 +3489,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -3491,10 +3500,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -3502,10 +3511,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -3513,10 +3522,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -3524,10 +3533,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -3535,10 +3544,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -3546,10 +3555,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -3557,10 +3566,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>419</v>
+        <v>114</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -3568,10 +3577,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
@@ -3579,10 +3588,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>125</v>
+        <v>420</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -3590,10 +3599,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
@@ -3601,7 +3610,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>421</v>
@@ -3612,10 +3621,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -3623,10 +3632,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
@@ -3634,10 +3643,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
@@ -3645,10 +3654,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>128</v>
+        <v>424</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
@@ -3656,7 +3665,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>128</v>
@@ -3667,10 +3676,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>425</v>
+        <v>128</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
@@ -3678,10 +3687,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>130</v>
+        <v>425</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -3689,10 +3698,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C142" s="1">
         <v>1</v>
@@ -3700,10 +3709,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
@@ -3711,10 +3720,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>426</v>
+        <v>128</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
@@ -3722,10 +3731,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>134</v>
+        <v>426</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
@@ -3733,10 +3742,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C146" s="1">
         <v>1</v>
@@ -3744,10 +3753,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
@@ -3755,10 +3764,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
@@ -3766,10 +3775,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>427</v>
+        <v>128</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
@@ -3777,10 +3786,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>130</v>
+        <v>427</v>
       </c>
       <c r="C150" s="1">
         <v>1</v>
@@ -3788,10 +3797,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C151" s="1">
         <v>1</v>
@@ -3799,10 +3808,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C152" s="1">
         <v>1</v>
@@ -3810,10 +3819,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C153" s="1">
         <v>1</v>
@@ -3821,10 +3830,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>426</v>
+        <v>128</v>
       </c>
       <c r="C154" s="1">
         <v>1</v>
@@ -3832,10 +3841,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>134</v>
+        <v>426</v>
       </c>
       <c r="C155" s="1">
         <v>1</v>
@@ -3843,10 +3852,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>428</v>
+        <v>134</v>
       </c>
       <c r="C156" s="1">
         <v>1</v>
@@ -3854,10 +3863,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>136</v>
+        <v>428</v>
       </c>
       <c r="C157" s="1">
         <v>1</v>
@@ -3865,10 +3874,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C158" s="1">
         <v>1</v>
@@ -3876,10 +3885,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C159" s="1">
         <v>1</v>
@@ -3887,10 +3896,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C160" s="1">
         <v>1</v>
@@ -3898,10 +3907,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C161" s="1">
         <v>1</v>
@@ -3909,10 +3918,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C162" s="1">
         <v>1</v>
@@ -3920,10 +3929,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
@@ -3931,10 +3940,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C164" s="1">
         <v>1</v>
@@ -3942,10 +3951,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C165" s="1">
         <v>1</v>
@@ -3953,10 +3962,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -3964,10 +3973,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>429</v>
+        <v>126</v>
       </c>
       <c r="C167" s="1">
         <v>1</v>
@@ -3975,10 +3984,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C168" s="1">
         <v>1</v>
@@ -3986,10 +3995,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>143</v>
+        <v>430</v>
       </c>
       <c r="C169" s="1">
         <v>1</v>
@@ -3997,10 +4006,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="C170" s="1">
         <v>1</v>
@@ -4008,7 +4017,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>108</v>
@@ -4019,7 +4028,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>108</v>
@@ -4030,7 +4039,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>108</v>
@@ -4041,7 +4050,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>108</v>
@@ -4052,7 +4061,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>108</v>
@@ -4063,7 +4072,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>108</v>
@@ -4074,7 +4083,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>108</v>
@@ -4085,10 +4094,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="C178" s="1">
         <v>1</v>
@@ -4096,10 +4105,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C179" s="1">
         <v>1</v>
@@ -4107,7 +4116,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>421</v>
@@ -4118,10 +4127,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C181" s="1">
         <v>1</v>
@@ -4129,10 +4138,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C182" s="1">
         <v>1</v>
@@ -4140,10 +4149,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>125</v>
+        <v>423</v>
       </c>
       <c r="C183" s="1">
         <v>1</v>
@@ -4151,10 +4160,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C184" s="1">
         <v>1</v>
@@ -4162,7 +4171,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>421</v>
@@ -4173,7 +4182,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>421</v>
@@ -4184,7 +4193,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>421</v>
@@ -4195,10 +4204,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>125</v>
+        <v>421</v>
       </c>
       <c r="C188" s="1">
         <v>1</v>
@@ -4206,10 +4215,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C189" s="1">
         <v>1</v>
@@ -4217,7 +4226,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>421</v>
@@ -4228,7 +4237,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>421</v>
@@ -4239,7 +4248,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>421</v>
@@ -4250,10 +4259,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>125</v>
+        <v>421</v>
       </c>
       <c r="C193" s="1">
         <v>1</v>
@@ -4261,10 +4270,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C194" s="1">
         <v>1</v>
@@ -4272,7 +4281,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>421</v>
@@ -4283,7 +4292,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>421</v>
@@ -4294,7 +4303,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>421</v>
@@ -4305,10 +4314,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>125</v>
+        <v>421</v>
       </c>
       <c r="C198" s="1">
         <v>1</v>
@@ -4316,10 +4325,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C199" s="1">
         <v>1</v>
@@ -4327,7 +4336,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>421</v>
@@ -4338,7 +4347,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>421</v>
@@ -4349,7 +4358,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>421</v>
@@ -4360,10 +4369,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>125</v>
+        <v>421</v>
       </c>
       <c r="C203" s="1">
         <v>1</v>
@@ -4371,10 +4380,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>421</v>
+        <v>125</v>
       </c>
       <c r="C204" s="1">
         <v>1</v>
@@ -4382,7 +4391,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>421</v>
@@ -4393,7 +4402,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>421</v>
@@ -4404,7 +4413,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>421</v>
@@ -4415,7 +4424,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>421</v>
@@ -4426,7 +4435,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>421</v>
@@ -4437,7 +4446,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>421</v>
@@ -4448,7 +4457,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>421</v>
@@ -4459,7 +4468,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>421</v>
@@ -4470,7 +4479,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>421</v>
@@ -4481,7 +4490,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>421</v>
@@ -4492,7 +4501,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>421</v>
@@ -4503,10 +4512,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="C216" s="1">
         <v>1</v>
@@ -4514,10 +4523,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C217" s="1">
         <v>1</v>
@@ -4525,10 +4534,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C218" s="1">
         <v>1</v>
@@ -4536,10 +4545,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C219" s="1">
         <v>1</v>
@@ -4547,10 +4556,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C220" s="1">
         <v>1</v>
@@ -4558,10 +4567,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C221" s="1">
         <v>1</v>
@@ -4569,10 +4578,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C222" s="1">
         <v>1</v>
@@ -4580,10 +4589,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C223" s="1">
         <v>1</v>
@@ -4591,10 +4600,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C224" s="1">
         <v>1</v>
@@ -4602,10 +4611,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C225" s="1">
         <v>1</v>
@@ -4613,7 +4622,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>439</v>
@@ -4624,10 +4633,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C227" s="1">
         <v>1</v>
@@ -4635,10 +4644,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C228" s="1">
         <v>1</v>
@@ -4646,10 +4655,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C229" s="1">
         <v>1</v>
@@ -4657,10 +4666,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C230" s="1">
         <v>1</v>
@@ -4668,7 +4677,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>443</v>
@@ -4679,10 +4688,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C232" s="1">
         <v>1</v>
@@ -4690,10 +4699,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C233" s="1">
         <v>1</v>
@@ -4701,10 +4710,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C234" s="1">
         <v>1</v>
@@ -4712,10 +4721,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C235" s="1">
         <v>1</v>
@@ -4723,10 +4732,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C236" s="1">
         <v>1</v>
@@ -4734,10 +4743,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C237" s="1">
         <v>1</v>
@@ -4745,10 +4754,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C238" s="1">
         <v>1</v>
@@ -4756,10 +4765,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C239" s="1">
         <v>1</v>
@@ -4767,10 +4776,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C240" s="1">
         <v>1</v>
@@ -4778,7 +4787,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>439</v>
@@ -4789,7 +4798,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>439</v>
@@ -4800,7 +4809,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>439</v>
@@ -4811,10 +4820,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="C244" s="1">
         <v>1</v>
@@ -4822,10 +4831,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C245" s="1">
         <v>1</v>
@@ -4833,7 +4842,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>452</v>
@@ -4844,7 +4853,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>452</v>
@@ -4855,7 +4864,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>452</v>
@@ -4866,10 +4875,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C249" s="1">
         <v>1</v>
@@ -4877,10 +4886,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C250" s="1">
         <v>1</v>
@@ -4888,7 +4897,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>454</v>
@@ -4899,10 +4908,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C252" s="1">
         <v>1</v>
@@ -4910,10 +4919,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C253" s="1">
         <v>1</v>
@@ -4921,10 +4930,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C254" s="1">
         <v>1</v>
@@ -4932,10 +4941,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C255" s="1">
         <v>1</v>
@@ -4943,10 +4952,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C256" s="1">
         <v>1</v>
@@ -4954,10 +4963,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C257" s="1">
         <v>1</v>
@@ -4965,10 +4974,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C258" s="1">
         <v>1</v>
@@ -4976,10 +4985,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C259" s="1">
         <v>1</v>
@@ -4987,10 +4996,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C260" s="1">
         <v>1</v>
@@ -4998,7 +5007,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>463</v>
@@ -5009,10 +5018,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C262" s="1">
         <v>1</v>
@@ -5020,10 +5029,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C263" s="1">
         <v>1</v>
@@ -5031,10 +5040,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C264" s="1">
         <v>1</v>
@@ -5042,10 +5051,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C265" s="1">
         <v>1</v>
@@ -5053,10 +5062,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C266" s="1">
         <v>1</v>
@@ -5064,10 +5073,10 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C267" s="1">
         <v>1</v>
@@ -5075,10 +5084,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C268" s="1">
         <v>1</v>
@@ -5086,10 +5095,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C269" s="1">
         <v>1</v>
@@ -5097,10 +5106,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C270" s="1">
         <v>1</v>
@@ -5108,7 +5117,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>472</v>
@@ -5119,10 +5128,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C272" s="1">
         <v>1</v>
@@ -5130,10 +5139,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C273" s="1">
         <v>1</v>
@@ -5141,10 +5150,10 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C274" s="1">
         <v>1</v>
@@ -5152,10 +5161,10 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C275" s="1">
         <v>1</v>
@@ -5163,10 +5172,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C276" s="1">
         <v>1</v>
@@ -5174,10 +5183,10 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C277" s="1">
         <v>1</v>
@@ -5185,10 +5194,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C278" s="1">
         <v>1</v>
@@ -5196,10 +5205,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C279" s="1">
         <v>1</v>
@@ -5207,10 +5216,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C280" s="1">
         <v>1</v>
@@ -5218,7 +5227,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>481</v>
@@ -5229,10 +5238,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C282" s="1">
         <v>1</v>
@@ -5240,10 +5249,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C283" s="1">
         <v>1</v>
@@ -5251,10 +5260,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C284" s="1">
         <v>1</v>
@@ -5262,10 +5271,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C285" s="1">
         <v>1</v>
@@ -5273,10 +5282,10 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C286" s="1">
         <v>1</v>
@@ -5284,10 +5293,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C287" s="1">
         <v>1</v>
@@ -5295,10 +5304,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C288" s="1">
         <v>1</v>
@@ -5306,10 +5315,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C289" s="1">
         <v>1</v>
@@ -5317,10 +5326,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C290" s="1">
         <v>1</v>
@@ -5328,7 +5337,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>490</v>
@@ -5339,10 +5348,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C292" s="1">
         <v>1</v>
@@ -5350,10 +5359,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C293" s="1">
         <v>1</v>
@@ -5361,10 +5370,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C294" s="1">
         <v>1</v>
@@ -5372,10 +5381,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C295" s="1">
         <v>1</v>
@@ -5383,10 +5392,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C296" s="1">
         <v>1</v>
@@ -5394,10 +5403,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C297" s="1">
         <v>1</v>
@@ -5405,10 +5414,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C298" s="1">
         <v>1</v>
@@ -5416,10 +5425,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C299" s="1">
         <v>1</v>
@@ -5427,10 +5436,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C300" s="1">
         <v>1</v>
@@ -5438,10 +5447,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C301" s="1">
         <v>1</v>
@@ -5449,7 +5458,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>499</v>
@@ -5460,10 +5469,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C303" s="1">
         <v>1</v>
@@ -5471,10 +5480,10 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C304" s="1">
         <v>1</v>
@@ -5482,10 +5491,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C305" s="1">
         <v>1</v>
@@ -5493,10 +5502,10 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C306" s="1">
         <v>1</v>
@@ -5504,10 +5513,10 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C307" s="1">
         <v>1</v>
@@ -5515,10 +5524,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C308" s="1">
         <v>1</v>
@@ -5526,10 +5535,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C309" s="1">
         <v>1</v>
@@ -5537,10 +5546,10 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>403</v>
+        <v>505</v>
       </c>
       <c r="C310" s="1">
         <v>1</v>
@@ -5548,10 +5557,10 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C311" s="1">
         <v>1</v>
@@ -5559,10 +5568,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C312" s="1">
         <v>1</v>
@@ -5570,7 +5579,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>0</v>
@@ -5581,10 +5590,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C314" s="1">
         <v>1</v>
@@ -5592,7 +5601,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>3</v>
@@ -5603,10 +5612,10 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>404</v>
+        <v>3</v>
       </c>
       <c r="C316" s="1">
         <v>1</v>
@@ -5614,10 +5623,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="C317" s="1">
         <v>1</v>
@@ -5625,7 +5634,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>0</v>
@@ -5636,10 +5645,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C319" s="1">
         <v>1</v>
@@ -5647,7 +5656,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>3</v>
@@ -5658,10 +5667,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>497</v>
+        <v>3</v>
       </c>
       <c r="C321" s="1">
         <v>1</v>
@@ -5669,10 +5678,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="C322" s="1">
         <v>1</v>
@@ -5680,10 +5689,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C323" s="1">
         <v>1</v>
@@ -5691,7 +5700,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>507</v>
@@ -5702,10 +5711,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C325" s="1">
         <v>1</v>
@@ -5713,10 +5722,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C326" s="1">
         <v>1</v>
@@ -5724,10 +5733,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C327" s="1">
         <v>1</v>
@@ -5735,10 +5744,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C328" s="1">
         <v>1</v>
@@ -5746,10 +5755,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C329" s="1">
         <v>1</v>
@@ -5757,10 +5766,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C330" s="1">
         <v>1</v>
@@ -5768,10 +5777,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C331" s="1">
         <v>1</v>
@@ -5779,10 +5788,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C332" s="1">
         <v>1</v>
@@ -5790,10 +5799,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C333" s="1">
         <v>1</v>
@@ -5801,10 +5810,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C334" s="1">
         <v>1</v>
@@ -5812,10 +5821,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C335" s="1">
         <v>1</v>
@@ -5823,10 +5832,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C336" s="1">
         <v>1</v>
@@ -5834,10 +5843,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C337" s="1">
         <v>1</v>
@@ -5845,10 +5854,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C338" s="1">
         <v>1</v>
@@ -5856,10 +5865,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C339" s="1">
         <v>1</v>
@@ -5867,10 +5876,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C340" s="1">
         <v>1</v>
@@ -5878,10 +5887,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C341" s="1">
         <v>1</v>
@@ -5889,10 +5898,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C342" s="1">
         <v>1</v>
@@ -5900,10 +5909,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C343" s="1">
         <v>1</v>
@@ -5911,10 +5920,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C344" s="1">
         <v>1</v>
@@ -5922,7 +5931,7 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>523</v>
@@ -5933,10 +5942,10 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C346" s="1">
         <v>1</v>
@@ -5944,10 +5953,10 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C347" s="1">
         <v>1</v>
@@ -5955,10 +5964,10 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C348" s="1">
         <v>1</v>
@@ -5966,10 +5975,10 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C349" s="1">
         <v>1</v>
@@ -5977,10 +5986,10 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C350" s="1">
         <v>1</v>
@@ -5988,10 +5997,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C351" s="1">
         <v>1</v>
@@ -5999,10 +6008,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C352" s="1">
         <v>1</v>
@@ -6010,10 +6019,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>497</v>
+        <v>529</v>
       </c>
       <c r="C353" s="1">
         <v>1</v>
@@ -6021,10 +6030,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="C354" s="1">
         <v>1</v>
@@ -6032,10 +6041,10 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="C355" s="1">
         <v>1</v>
@@ -6043,7 +6052,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>499</v>
@@ -6054,10 +6063,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C357" s="1">
         <v>1</v>
@@ -6065,7 +6074,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>504</v>
@@ -6076,10 +6085,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C359" s="1">
         <v>1</v>
@@ -6087,10 +6096,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C360" s="1">
         <v>1</v>
@@ -6098,7 +6107,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>503</v>
@@ -6109,10 +6118,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="C362" s="1">
         <v>1</v>
@@ -6120,7 +6129,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>510</v>
@@ -6131,10 +6140,10 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="C364" s="1">
         <v>1</v>
@@ -6142,10 +6151,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C365" s="1">
         <v>1</v>
@@ -6153,10 +6162,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C366" s="1">
         <v>1</v>
@@ -6164,7 +6173,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>532</v>
@@ -6175,10 +6184,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C368" s="1">
         <v>1</v>
@@ -6186,10 +6195,10 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C369" s="1">
         <v>1</v>
@@ -6197,10 +6206,10 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C370" s="1">
         <v>1</v>
@@ -6208,10 +6217,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C371" s="1">
         <v>1</v>
@@ -6219,10 +6228,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C372" s="1">
         <v>1</v>
@@ -6230,10 +6239,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C373" s="1">
         <v>1</v>
@@ -6241,10 +6250,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C374" s="1">
         <v>1</v>
@@ -6252,10 +6261,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C375" s="1">
         <v>1</v>
@@ -6263,21 +6272,21 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C376" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>308</v>
+        <v>541</v>
       </c>
       <c r="C377" s="1">
         <v>7</v>
@@ -6285,10 +6294,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>542</v>
+        <v>308</v>
       </c>
       <c r="C378" s="1">
         <v>7</v>
@@ -6296,43 +6305,43 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>405</v>
+        <v>309</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>406</v>
+        <v>542</v>
       </c>
       <c r="C379" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>543</v>
+        <v>406</v>
       </c>
       <c r="C380" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B381" s="1">
-        <v>1</v>
+        <v>407</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="C381" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B382" s="1" t="s">
         <v>393</v>
+      </c>
+      <c r="B382" s="1">
+        <v>2</v>
       </c>
       <c r="C382" s="1">
         <v>2</v>
@@ -6340,13 +6349,46 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B383" s="1">
-        <v>1</v>
+        <v>394</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="C383" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B384" s="1">
+        <v>2</v>
+      </c>
+      <c r="C384" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C385" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C386" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>